<commit_message>
added dynamic hashtable functionality -gerard
</commit_message>
<xml_diff>
--- a/src/test/java/gerard/resources/excel/testdata.xlsx
+++ b/src/test/java/gerard/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grecinto\Desktop\testLearning\src\test\java\gerard\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{105C5DFB-263E-4FB2-B69C-46CD8F2E0A76}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EE6750E7-26D7-4DC5-849C-1E1BA5B7FF7F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{070B1EE3-25CE-48A7-9212-1969A4600F02}"/>
   </bookViews>
@@ -36,10 +36,10 @@
     <t>postcode</t>
   </si>
   <si>
-    <t>firstTest</t>
+    <t>gdsfsd</t>
   </si>
   <si>
-    <t>lastTest</t>
+    <t>sdfsdfsdf</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>